<commit_message>
Changed master_sheet to final_merge
</commit_message>
<xml_diff>
--- a/server/master_sheet.xlsx
+++ b/server/master_sheet.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="8_{148DB330-9CF6-436A-8896-3817F9E77B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8705F7BF-3409-48AC-B784-7569F112F956}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2616" yWindow="2616" windowWidth="18276" windowHeight="9912" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Data" sheetId="1" r:id="rId1"/>
@@ -391,6 +391,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -682,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="96" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,6 +1135,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="67a8f749-7263-4126-9cf2-3ace36dd08d6" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ded1046d-9b62-4234-9080-a2f50b012ab9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010012CADD28B1E4AD4280BC6F9880014CBF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a09c7a73af476929d2f900da0d352180">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ded1046d-9b62-4234-9080-a2f50b012ab9" xmlns:ns3="67a8f749-7263-4126-9cf2-3ace36dd08d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ba97e7e780f0cae3f5157d241f876312" ns2:_="" ns3:_="">
     <xsd:import namespace="ded1046d-9b62-4234-9080-a2f50b012ab9"/>
@@ -1365,17 +1380,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="67a8f749-7263-4126-9cf2-3ace36dd08d6" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ded1046d-9b62-4234-9080-a2f50b012ab9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3032DCEC-B7AE-4ED6-9938-633CDA03B71B}">
   <ds:schemaRefs>
@@ -1385,6 +1389,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{441025C5-4796-4F77-9D16-5328B45992C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="67a8f749-7263-4126-9cf2-3ace36dd08d6"/>
+    <ds:schemaRef ds:uri="ded1046d-9b62-4234-9080-a2f50b012ab9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3A59E8-996E-4613-B2A2-E1812F94A26F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1401,15 +1416,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{441025C5-4796-4F77-9D16-5328B45992C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="67a8f749-7263-4126-9cf2-3ace36dd08d6"/>
-    <ds:schemaRef ds:uri="ded1046d-9b62-4234-9080-a2f50b012ab9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changed to a different template, changed undefined to N/A and added new column values to populate
</commit_message>
<xml_diff>
--- a/server/master_sheet.xlsx
+++ b/server/master_sheet.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="8_{148DB330-9CF6-436A-8896-3817F9E77B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8705F7BF-3409-48AC-B784-7569F112F956}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2616" yWindow="2616" windowWidth="18276" windowHeight="9912" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="768" yWindow="768" windowWidth="15732" windowHeight="9912" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Data" sheetId="1" r:id="rId1"/>
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="96" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1135,17 +1135,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="67a8f749-7263-4126-9cf2-3ace36dd08d6" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ded1046d-9b62-4234-9080-a2f50b012ab9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010012CADD28B1E4AD4280BC6F9880014CBF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a09c7a73af476929d2f900da0d352180">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ded1046d-9b62-4234-9080-a2f50b012ab9" xmlns:ns3="67a8f749-7263-4126-9cf2-3ace36dd08d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ba97e7e780f0cae3f5157d241f876312" ns2:_="" ns3:_="">
     <xsd:import namespace="ded1046d-9b62-4234-9080-a2f50b012ab9"/>
@@ -1380,6 +1369,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="67a8f749-7263-4126-9cf2-3ace36dd08d6" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ded1046d-9b62-4234-9080-a2f50b012ab9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3032DCEC-B7AE-4ED6-9938-633CDA03B71B}">
   <ds:schemaRefs>
@@ -1389,17 +1389,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{441025C5-4796-4F77-9D16-5328B45992C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="67a8f749-7263-4126-9cf2-3ace36dd08d6"/>
-    <ds:schemaRef ds:uri="ded1046d-9b62-4234-9080-a2f50b012ab9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3A59E8-996E-4613-B2A2-E1812F94A26F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1416,4 +1405,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{441025C5-4796-4F77-9D16-5328B45992C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="67a8f749-7263-4126-9cf2-3ace36dd08d6"/>
+    <ds:schemaRef ds:uri="ded1046d-9b62-4234-9080-a2f50b012ab9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>